<commit_message>
Created new branch and pushed code
</commit_message>
<xml_diff>
--- a/ExcelFiles/Automated_SmokeTest_Result.xlsx
+++ b/ExcelFiles/Automated_SmokeTest_Result.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,6 +84,12 @@
       <sz val="16"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -117,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -150,6 +156,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -536,33 +543,33 @@
   </sheetPr>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col width="49.77734375" customWidth="1" style="15" min="1" max="1"/>
-    <col width="75.5546875" customWidth="1" style="15" min="2" max="2"/>
-    <col width="63.88671875" customWidth="1" style="15" min="3" max="3"/>
-    <col width="13.21875" customWidth="1" style="15" min="4" max="4"/>
-    <col width="21.5546875" customWidth="1" style="15" min="5" max="5"/>
+    <col width="49.77734375" customWidth="1" style="16" min="1" max="1"/>
+    <col width="96.44140625" customWidth="1" style="16" min="2" max="2"/>
+    <col width="101.6640625" customWidth="1" style="16" min="3" max="3"/>
+    <col width="13.21875" customWidth="1" style="16" min="4" max="4"/>
+    <col width="21.5546875" customWidth="1" style="16" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25.8" customHeight="1" s="15">
-      <c r="A1" s="16" t="inlineStr">
+    <row r="1" ht="25.8" customHeight="1" s="16">
+      <c r="A1" s="17" t="inlineStr">
         <is>
           <t>CROWD - Smoket Testing Result For Test Environment On</t>
         </is>
       </c>
       <c r="C1" s="13" t="inlineStr">
         <is>
-          <t>12/03/2024 12:48:PM</t>
+          <t>20/05/2024 08:23:AM</t>
         </is>
       </c>
       <c r="D1" s="12" t="n"/>
     </row>
-    <row r="3" ht="18" customHeight="1" s="15">
+    <row r="3" ht="18" customHeight="1" s="16">
       <c r="A3" s="10" t="inlineStr">
         <is>
           <t>Functionality</t>
@@ -584,20 +591,20 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="18" customHeight="1" s="15">
+    <row r="4" ht="18" customHeight="1" s="16">
       <c r="A4" s="5" t="n"/>
       <c r="B4" s="2" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
     </row>
-    <row r="5" ht="18" customHeight="1" s="15">
-      <c r="A5" s="14" t="inlineStr">
+    <row r="5" ht="18" customHeight="1" s="16">
+      <c r="A5" s="15" t="inlineStr">
         <is>
           <t>Verifying  LOGO &amp; TITLE</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="15.6" customHeight="1" s="15">
+    <row r="6" ht="15.6" customHeight="1" s="16">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>CMS - Homepage Header Logo/ Main Logo</t>
@@ -615,10 +622,10 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="15.6" customHeight="1" s="15">
+    <row r="7" ht="15.6" customHeight="1" s="16">
       <c r="A7" s="1" t="n"/>
     </row>
-    <row r="8" ht="15.6" customHeight="1" s="15">
+    <row r="8" ht="15.6" customHeight="1" s="16">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Main Title</t>
@@ -702,7 +709,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="99" customHeight="1" s="15">
+    <row r="16" ht="99" customHeight="1" s="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
           <t>CROWD Summary</t>
@@ -727,14 +734,14 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="18" customHeight="1" s="15">
-      <c r="A18" s="14" t="inlineStr">
+    <row r="18" ht="18" customHeight="1" s="16">
+      <c r="A18" s="15" t="inlineStr">
         <is>
           <t>Verifying File Submission</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="42.6" customHeight="1" s="15">
+    <row r="20" ht="42.6" customHeight="1" s="16">
       <c r="A20" s="9" t="inlineStr">
         <is>
           <t>File Instructions</t>
@@ -756,7 +763,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="15.6" customHeight="1" s="15">
+    <row r="22" ht="15.6" customHeight="1" s="16">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>Uploaded File Name &amp; Filename displayed on Status</t>
@@ -764,12 +771,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CONTRACTOR_MAPPING_VALIDATION_BAD_BSI_FORM_S.txt</t>
+          <t>9_INVALID_ROWS_FORM_S.txt</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CONTRACTOR_MAPPING_VALIDATION_BAD_BSI_FORM_S.txt</t>
+          <t>9_INVALID_ROWS_FORM_S.txt</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -778,10 +785,10 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="15.6" customHeight="1" s="15">
+    <row r="23" ht="15.6" customHeight="1" s="16">
       <c r="A23" s="1" t="n"/>
     </row>
-    <row r="24" ht="15.6" customHeight="1" s="15">
+    <row r="24" ht="15.6" customHeight="1" s="16">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>Comment Entered &amp; Comment displayed</t>
@@ -789,12 +796,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BAD_BSI</t>
+          <t>Invalid Rows</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>BAD_BSI</t>
+          <t>Invalid Rows</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -803,10 +810,10 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="15.6" customHeight="1" s="15">
+    <row r="25" ht="15.6" customHeight="1" s="16">
       <c r="A25" s="1" t="n"/>
     </row>
-    <row r="26" ht="15.6" customHeight="1" s="15">
+    <row r="26" ht="15.6" customHeight="1" s="16">
       <c r="A26" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
@@ -814,12 +821,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>03/12/2024 12:49 PM</t>
+          <t>05/20/2024 08:24 AM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>03/12/2024 12:49 PM</t>
+          <t>05/20/2024 08:24 AM</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -828,27 +835,27 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="18" customHeight="1" s="15">
-      <c r="A28" s="14" t="inlineStr">
-        <is>
-          <t>Verifying 'DASHBOARD' Page's First Record &amp; MicroStrategy Title</t>
+    <row r="28" ht="18" customHeight="1" s="16">
+      <c r="A28" s="15" t="inlineStr">
+        <is>
+          <t>Verifying 'TABLE' Page's First Record &amp; MicroStrategy Title</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Dashboard ID</t>
+          <t>Table ID</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>B01 PART B</t>
+          <t>UTBL01</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>B01 PART B</t>
+          <t>UTBL01</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -860,17 +867,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Dashboard Name</t>
+          <t>Table Type</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>WORKLOAD OPERATIONS: CLAIMS RECEIVED, PROCESSED AND PENDING</t>
+          <t>PART B</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>WORKLOAD OPERATIONS: CLAIMS RECEIVED, PROCESSED AND PENDING</t>
+          <t>PART B</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -882,17 +889,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Dashboard Description</t>
+          <t>Table Name</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>WORKLOAD OPERATIONS: CLAIMS RECEIVED, PROCESSED, AND PENDING DATA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>WORKLOAD OPERATIONS: CLAIMS RECEIVED, PROCESSED, AND PENDING DATA</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -909,22 +916,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>B01. MicroStrategy</t>
+          <t>(UTBL01 - PART B) WORKLOAD OPERATIONS: CLAIMS RECEIVED, PROCESSED, AND PENDING DATA. MicroStrategy</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>B01. MicroStrategy</t>
+          <t>(UTBL01 - PART B) WORKLOAD OPERATIONS: CLAIMS RECEIVED, PROCESSED, AND PENDING DATA. MicroStrategy</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" ht="18" customHeight="1" s="15">
-      <c r="A39" s="14" t="inlineStr">
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="18" customHeight="1" s="16">
+      <c r="A39" s="15" t="inlineStr">
         <is>
           <t>Verifying 'FORM' Page's First Record &amp; MicroStrategey Title</t>
         </is>
@@ -938,15 +945,15 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>FORM 7A</t>
+          <t>FORM 7</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FORM 7A</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
+          <t>FORM 7</t>
+        </is>
+      </c>
+      <c r="D41" s="14" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -987,12 +994,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>APPEALS ACTIVITY CMS-2592</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Pass</t>
+          <t>APPEALS ACTIVITY (CMS-2592)</t>
         </is>
       </c>
     </row>
@@ -1018,10 +1020,10 @@
         </is>
       </c>
     </row>
-    <row r="50" ht="18" customHeight="1" s="15">
-      <c r="A50" s="14" t="inlineStr">
-        <is>
-          <t>Verifying 'REPORT' Page's First Record &amp; MicroStrategey Title</t>
+    <row r="50" ht="18" customHeight="1" s="16">
+      <c r="A50" s="15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Verifying 'REPORT' Page's First Record </t>
         </is>
       </c>
     </row>
@@ -1033,12 +1035,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>URPT-CFS</t>
+          <t>URPT01</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>URPT-CFS</t>
+          <t>URPT01</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1055,21 +1057,21 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>CROWD FILE STATUS</t>
+          <t>CONTRACTOR MAPPING</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CROWD FILE STATUS</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row r="56" ht="43.2" customHeight="1" s="15">
+          <t>CONTRACTOR MAPPING</t>
+        </is>
+      </c>
+      <c r="D54" s="14" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="18.6" customHeight="1" s="16">
       <c r="A56" t="inlineStr">
         <is>
           <t>Report Description</t>
@@ -1077,12 +1079,12 @@
       </c>
       <c r="B56" s="7" t="inlineStr">
         <is>
-          <t>This report lists the current status of, and other details relating to, the data file submissions for the CROWD Forms based on the due date(s) for the respective reporting period(s) specified.</t>
+          <t>This report lists all CROWD Contractor Details including their roles.</t>
         </is>
       </c>
       <c r="C56" s="7" t="inlineStr">
         <is>
-          <t>This report lists the current status of, and other details relating to, the data file submissions for the CROWD Forms based on the due date(s) for the respective reporting period(s) specified.</t>
+          <t>This report lists all CROWD Contractor Details including their roles.</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1091,10 +1093,10 @@
         </is>
       </c>
     </row>
-    <row r="58" ht="17.4" customHeight="1" s="15">
-      <c r="A58" s="14" t="inlineStr">
-        <is>
-          <t>Verifying 'Resources' Page</t>
+    <row r="58" ht="17.4" customHeight="1" s="16">
+      <c r="A58" s="15" t="inlineStr">
+        <is>
+          <t>Verifying 'Resources' Page's First Record</t>
         </is>
       </c>
     </row>
@@ -1164,10 +1166,10 @@
         </is>
       </c>
     </row>
-    <row r="67" ht="18" customHeight="1" s="15">
-      <c r="A67" s="14" t="inlineStr">
-        <is>
-          <t>Verifying 'NEWS' Page</t>
+    <row r="67" ht="18" customHeight="1" s="16">
+      <c r="A67" s="15" t="inlineStr">
+        <is>
+          <t>Verifying 'NEWS' Page For Year 2020</t>
         </is>
       </c>
     </row>
@@ -1179,12 +1181,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Attn: Medicare Contractors | February 12, 2020</t>
+          <t>Attn: ALL CROWD Users | October 1, 2024</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Attn: Medicare Contractors | February 12, 2020</t>
+          <t>Attn: ALL CROWD Users | October 1, 2024</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1193,16 +1195,15 @@
         </is>
       </c>
     </row>
-    <row r="70" ht="72" customHeight="1" s="15">
-      <c r="B70" s="7" t="inlineStr">
-        <is>
-          <t>Although CR 11353 (Supplier Specialty Code D5) for Medicare Workload Data
- Reporting (MWDR) in calendar year 2022. Please email both Steve Calfo via Stephen.Calfo@cms.hhs.gov and Tonya Neal via Tonya.Neal@cms.hhs.gov if you have any questions or concerns.</t>
+    <row r="70" ht="33.6" customHeight="1" s="16">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>This is a placeholder. This will be updated closer to the Go Live Date.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Although CR 11353 (Supplier Specialty Code D5) for Medicare Workload Data Reporting (MWDR) in calendar year 2022. Please email both Steve Calfo via Stephen.Calfo@cms.hhs.gov and Tonya Neal via Tonya.Neal@cms.hhs.gov if you have any questions or concerns.</t>
+          <t>This is a placeholder. This will be updated closer to the Go Live Date.</t>
         </is>
       </c>
     </row>

</xml_diff>